<commit_message>
working on excel reader and adding extend report (extend report needs to be corrected - was made according to tutorial on usemy and needs to be corrected - there is no catching for skipped/failed tests currently)
</commit_message>
<xml_diff>
--- a/src/test/resources/testData.xlsx
+++ b/src/test/resources/testData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafi\Desktop\travel2\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379AF055-6DF4-4ADB-95BB-2E902DC43CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DACCAB6-10C6-4487-A1E0-D56992DDE1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>city</t>
   </si>
@@ -39,15 +39,26 @@
     <t>Dubai</t>
   </si>
   <si>
-    <t>xxx</t>
+    <t>Grand Plaza Apartments</t>
+  </si>
+  <si>
+    <t>Jumeirah Beach Hotel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -75,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,7 +389,7 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -386,10 +398,11 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>